<commit_message>
Remove tmp file and latest update to the results file.
</commit_message>
<xml_diff>
--- a/src/experiments/results/run-2024.02.24/results_with_evaluation.xlsx
+++ b/src/experiments/results/run-2024.02.24/results_with_evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savasp/dev/digital-twin/src/experiments/results/run-2024.02.24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A786178-6BF6-1140-85F8-4BA2227D7134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1422C796-0F67-8747-A6A2-0C86034DF003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="33840" windowHeight="19460" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="33840" windowHeight="19460" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="webpages-linkedin_llama2-7b" sheetId="1" r:id="rId1"/>
@@ -5906,16 +5906,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10096,8 +10096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10733,6 +10733,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -10740,8 +10741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11377,6 +11378,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -12028,8 +12030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12665,6 +12667,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>